<commit_message>
parsed files now being zipped
</commit_message>
<xml_diff>
--- a/modules/Parse.xlsx
+++ b/modules/Parse.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>2013-09-18T17:15:12.000+03</t>
   </si>
@@ -33,31 +33,34 @@
     <t>collector</t>
   </si>
   <si>
+    <t>1379685996075.png</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Check ee sheet</t>
+  </si>
+  <si>
+    <t>Check dl sheet</t>
+  </si>
+  <si>
+    <t>Check bs sheet</t>
+  </si>
+  <si>
+    <t>Check hr sheet</t>
+  </si>
+  <si>
+    <t>Check ph sheet</t>
+  </si>
+  <si>
+    <t>Check ms sheet</t>
+  </si>
+  <si>
     <t>http://en.m.wikipedia.org</t>
-  </si>
-  <si>
-    <t>NULL</t>
-  </si>
-  <si>
-    <t>Thomas</t>
-  </si>
-  <si>
-    <t>Check ee sheet</t>
-  </si>
-  <si>
-    <t>Check dl sheet</t>
-  </si>
-  <si>
-    <t>Check bs sheet</t>
-  </si>
-  <si>
-    <t>Check hr sheet</t>
-  </si>
-  <si>
-    <t>Check ph sheet</t>
-  </si>
-  <si>
-    <t>Check ms sheet</t>
   </si>
   <si>
     <t>main_sheet (P1)</t>
@@ -714,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -808,19 +811,19 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F1">
         <v>12000</v>
@@ -829,27 +832,27 @@
         <v>15000</v>
       </c>
       <c r="H1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F2">
         <v>12000</v>
@@ -858,10 +861,10 @@
         <v>15000</v>
       </c>
       <c r="H2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -904,10 +907,10 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C1">
         <v>12</v>
@@ -919,18 +922,18 @@
         <v>21</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>12</v>
@@ -942,10 +945,10 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -996,16 +999,16 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1">
         <v>2</v>
@@ -1035,21 +1038,21 @@
         <v>3</v>
       </c>
       <c r="N1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -1079,21 +1082,21 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1123,21 +1126,21 @@
         <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -1167,7 +1170,7 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1224,144 +1227,144 @@
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R1" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" t="s">
-        <v>22</v>
-      </c>
       <c r="T1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>34</v>
+      </c>
+      <c r="S2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s">
         <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-      <c r="N2" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1400,50 +1403,50 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1482,50 +1485,50 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1564,66 +1567,66 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1672,31 +1675,31 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J1">
         <v>20000</v>
@@ -1705,39 +1708,39 @@
         <v>15000</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J2">
         <v>20000</v>
@@ -1746,10 +1749,10 @@
         <v>15000</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1788,18 +1791,18 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1845,16 +1848,16 @@
   <sheetData>
     <row r="1" spans="1:20">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E1">
         <v>11000</v>
@@ -1863,27 +1866,27 @@
         <v>12000</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>11000</v>
@@ -1892,13 +1895,13 @@
         <v>12000</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>